<commit_message>
Add header insert in dataframe
</commit_message>
<xml_diff>
--- a/Test/UnitTest/srcTest/dataFrameInsert.xlsx
+++ b/Test/UnitTest/srcTest/dataFrameInsert.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -26,7 +26,13 @@
     <t xml:space="preserve">col3</t>
   </si>
   <si>
+    <t xml:space="preserve">a1</t>
+  </si>
+  <si>
     <t xml:space="preserve">a3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
   </si>
 </sst>
 </file>
@@ -82,6 +88,9 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -90,7 +99,32 @@
         <v>4</v>
       </c>
       <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
         <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>8.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>